<commit_message>
rename controller and omit email to user model
</commit_message>
<xml_diff>
--- a/app/assets/test.xlsx
+++ b/app/assets/test.xlsx
@@ -44,6 +44,54 @@
   </si>
   <si>
     <t>honghong@gmail.com</t>
+  </si>
+  <si>
+    <t>경영학과</t>
+  </si>
+  <si>
+    <t>김민혁</t>
+  </si>
+  <si>
+    <t>01012341234</t>
+  </si>
+  <si>
+    <t>ha@gmail.com</t>
+  </si>
+  <si>
+    <t>경영학과</t>
+  </si>
+  <si>
+    <t>홍철주</t>
+  </si>
+  <si>
+    <t>01012341234</t>
+  </si>
+  <si>
+    <t>ha@gmail.com</t>
+  </si>
+  <si>
+    <t>경영학과</t>
+  </si>
+  <si>
+    <t>김영훈</t>
+  </si>
+  <si>
+    <t>01012341234</t>
+  </si>
+  <si>
+    <t>ha@gmail.com</t>
+  </si>
+  <si>
+    <t>경영학과</t>
+  </si>
+  <si>
+    <t>강성희</t>
+  </si>
+  <si>
+    <t>01012341234</t>
+  </si>
+  <si>
+    <t>ha@gmail.com</t>
   </si>
   <si>
     <t>경영학과</t>
@@ -163,16 +211,60 @@
       </c>
     </row>
     <row r="4">
-      <c s="2" r="B4"/>
+      <c t="s" s="1" r="A4">
+        <v>12</v>
+      </c>
+      <c t="s" s="3" r="B4">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="C4">
+        <v>14</v>
+      </c>
+      <c t="s" s="1" r="D4">
+        <v>15</v>
+      </c>
     </row>
     <row r="5">
-      <c s="2" r="B5"/>
+      <c t="s" s="1" r="A5">
+        <v>16</v>
+      </c>
+      <c t="s" s="3" r="B5">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="C5">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="D5">
+        <v>19</v>
+      </c>
     </row>
     <row r="6">
-      <c s="2" r="B6"/>
+      <c t="s" s="1" r="A6">
+        <v>20</v>
+      </c>
+      <c t="s" s="3" r="B6">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="C6">
+        <v>22</v>
+      </c>
+      <c t="s" s="1" r="D6">
+        <v>23</v>
+      </c>
     </row>
     <row r="7">
-      <c s="2" r="B7"/>
+      <c t="s" s="1" r="A7">
+        <v>24</v>
+      </c>
+      <c t="s" s="3" r="B7">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="C7">
+        <v>26</v>
+      </c>
+      <c t="s" s="1" r="D7">
+        <v>27</v>
+      </c>
     </row>
     <row r="8">
       <c s="2" r="B8"/>

</xml_diff>

<commit_message>
add column 'phonenumber' and 'major' to user
</commit_message>
<xml_diff>
--- a/app/assets/test.xlsx
+++ b/app/assets/test.xlsx
@@ -55,46 +55,46 @@
     <t>01012341234</t>
   </si>
   <si>
-    <t>ha@gmail.com</t>
+    <t>mk@gmail.com</t>
   </si>
   <si>
-    <t>경영학과</t>
+    <t>컴퓨터공학부</t>
   </si>
   <si>
     <t>홍철주</t>
   </si>
   <si>
-    <t>01012341234</t>
+    <t>01043214321</t>
   </si>
   <si>
-    <t>ha@gmail.com</t>
+    <t>fe@gmail.com</t>
   </si>
   <si>
-    <t>경영학과</t>
+    <t>수학과</t>
   </si>
   <si>
     <t>김영훈</t>
   </si>
   <si>
-    <t>01012341234</t>
+    <t>01012322222</t>
   </si>
   <si>
-    <t>ha@gmail.com</t>
+    <t>kim@gmail.com</t>
   </si>
   <si>
-    <t>경영학과</t>
+    <t>심리학과</t>
   </si>
   <si>
     <t>강성희</t>
   </si>
   <si>
-    <t>01012341234</t>
+    <t>01012343333</t>
   </si>
   <si>
-    <t>ha@gmail.com</t>
+    <t>kang@gmail.com</t>
   </si>
   <si>
-    <t>경영학과</t>
+    <t>경제학과</t>
   </si>
 </sst>
 </file>

</xml_diff>